<commit_message>
Gant-Übung in Netzplan_Übung2 FIAE D (Übung2)
</commit_message>
<xml_diff>
--- a/FIAED Übungen/Netzplan_Übung.xlsx
+++ b/FIAED Übungen/Netzplan_Übung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="29">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -114,9 +114,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -189,7 +191,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,7 +207,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -230,6 +232,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -277,7 +285,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -378,7 +386,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="80" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="80" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,7 +424,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Gesamtpuffer" xfId="20"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -452,6 +484,22 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -469,7 +517,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -502,7 +550,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -1069,13 +1117,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1084,7 +1132,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1084680" y="2601720"/>
+          <a:off x="1084680" y="2602080"/>
           <a:ext cx="0" cy="826200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1111,13 +1159,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1126,7 +1174,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2440440" y="3414600"/>
+          <a:off x="2440440" y="3414960"/>
           <a:ext cx="0" cy="826200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1153,13 +1201,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1168,7 +1216,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5151600" y="3414600"/>
+          <a:off x="5151600" y="3414960"/>
           <a:ext cx="0" cy="826200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1195,13 +1243,13 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1210,7 +1258,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6507360" y="2601720"/>
+          <a:off x="6507360" y="2602080"/>
           <a:ext cx="0" cy="826200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1240,15 +1288,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1257,7 +1305,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1082160" y="2588040"/>
+          <a:off x="1082520" y="2958840"/>
           <a:ext cx="0" cy="826200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1283,14 +1331,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>6120</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1299,7 +1347,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="811440" y="2600280"/>
+          <a:off x="811440" y="2970720"/>
           <a:ext cx="547200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1325,14 +1373,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:colOff>7560</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1341,7 +1389,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2163960" y="2600280"/>
+          <a:off x="2163960" y="2970720"/>
           <a:ext cx="547200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1372,7 +1420,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
@@ -1383,7 +1431,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2163960" y="3412800"/>
+          <a:off x="2163960" y="3791880"/>
           <a:ext cx="547200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1408,13 +1456,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>6480</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
@@ -1425,7 +1473,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3516480" y="3412800"/>
+          <a:off x="3515400" y="3791880"/>
           <a:ext cx="547200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1450,15 +1498,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:colOff>6480</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1467,7 +1515,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3516480" y="2600280"/>
+          <a:off x="3515400" y="2970720"/>
           <a:ext cx="547200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1492,15 +1540,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:colOff>6480</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1509,7 +1557,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4869000" y="2600280"/>
+          <a:off x="4867920" y="2970720"/>
           <a:ext cx="547200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1535,14 +1583,14 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>6480</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:colOff>6840</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1551,7 +1599,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6221880" y="2600280"/>
+          <a:off x="6220800" y="2970720"/>
           <a:ext cx="547200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1576,13 +1624,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>6480</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
@@ -1593,7 +1641,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4869000" y="3412800"/>
+          <a:off x="4867920" y="3791880"/>
           <a:ext cx="547200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1618,13 +1666,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>6480</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
@@ -1635,7 +1683,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1082160" y="3412800"/>
+          <a:off x="1082520" y="3791880"/>
           <a:ext cx="276480" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1666,7 +1714,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>6480</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
@@ -1677,7 +1725,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2434680" y="4234320"/>
+          <a:off x="2433600" y="4622400"/>
           <a:ext cx="276480" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1702,7 +1750,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>7920</xdr:rowOff>
     </xdr:from>
@@ -1719,7 +1767,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3516480" y="4234320"/>
+          <a:off x="3515400" y="4622400"/>
           <a:ext cx="276480" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1750,7 +1798,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>6480</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
@@ -1761,7 +1809,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5139720" y="4234320"/>
+          <a:off x="5138640" y="4622400"/>
           <a:ext cx="276480" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1792,7 +1840,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>6480</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
@@ -1803,7 +1851,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6221880" y="4234320"/>
+          <a:off x="6220800" y="4622400"/>
           <a:ext cx="276480" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1830,13 +1878,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1845,7 +1893,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2434680" y="3414600"/>
+          <a:off x="2433600" y="3794400"/>
           <a:ext cx="0" cy="826200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1872,13 +1920,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1887,7 +1935,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3787200" y="3414600"/>
+          <a:off x="3786120" y="3794400"/>
           <a:ext cx="0" cy="826200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1914,13 +1962,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1929,7 +1977,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5139720" y="3414600"/>
+          <a:off x="5138640" y="3794400"/>
           <a:ext cx="0" cy="826200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1956,13 +2004,13 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1971,7 +2019,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6492240" y="3414600"/>
+          <a:off x="6490800" y="3794400"/>
           <a:ext cx="0" cy="826200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1998,13 +2046,13 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2013,7 +2061,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6492240" y="2601720"/>
+          <a:off x="6490800" y="2972520"/>
           <a:ext cx="0" cy="826200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2040,13 +2088,13 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
+      <xdr:colOff>6120</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2055,7 +2103,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6221520" y="3413880"/>
+          <a:off x="6220440" y="3793320"/>
           <a:ext cx="276480" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2087,7 +2135,7 @@
   </sheetPr>
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -2876,18 +2924,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB28"/>
+  <dimension ref="A1:BX28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K10" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z22" activeCellId="0" sqref="Z22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="3.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="10" style="0" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="51" style="0" width="3.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2903,6 +2954,210 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="27" t="n">
+        <v>44536</v>
+      </c>
+      <c r="K1" s="27" t="n">
+        <v>44537</v>
+      </c>
+      <c r="L1" s="27" t="n">
+        <v>44538</v>
+      </c>
+      <c r="M1" s="27" t="n">
+        <v>44539</v>
+      </c>
+      <c r="N1" s="27" t="n">
+        <v>44540</v>
+      </c>
+      <c r="O1" s="27" t="n">
+        <v>44541</v>
+      </c>
+      <c r="P1" s="27" t="n">
+        <v>44542</v>
+      </c>
+      <c r="Q1" s="27" t="n">
+        <v>44543</v>
+      </c>
+      <c r="R1" s="27" t="n">
+        <v>44544</v>
+      </c>
+      <c r="S1" s="27" t="n">
+        <v>44545</v>
+      </c>
+      <c r="T1" s="27" t="n">
+        <v>44546</v>
+      </c>
+      <c r="U1" s="27" t="n">
+        <v>44547</v>
+      </c>
+      <c r="V1" s="27" t="n">
+        <v>44548</v>
+      </c>
+      <c r="W1" s="27" t="n">
+        <v>44549</v>
+      </c>
+      <c r="X1" s="27" t="n">
+        <v>44550</v>
+      </c>
+      <c r="Y1" s="27" t="n">
+        <v>44551</v>
+      </c>
+      <c r="Z1" s="27" t="n">
+        <v>44552</v>
+      </c>
+      <c r="AA1" s="27" t="n">
+        <v>44553</v>
+      </c>
+      <c r="AB1" s="28" t="n">
+        <v>44554</v>
+      </c>
+      <c r="AC1" s="27" t="n">
+        <v>44555</v>
+      </c>
+      <c r="AD1" s="27" t="n">
+        <v>44556</v>
+      </c>
+      <c r="AE1" s="27" t="n">
+        <v>44557</v>
+      </c>
+      <c r="AF1" s="27" t="n">
+        <v>44558</v>
+      </c>
+      <c r="AG1" s="27" t="n">
+        <v>44559</v>
+      </c>
+      <c r="AH1" s="27" t="n">
+        <v>44560</v>
+      </c>
+      <c r="AI1" s="28" t="n">
+        <v>44561</v>
+      </c>
+      <c r="AJ1" s="27" t="n">
+        <v>44562</v>
+      </c>
+      <c r="AK1" s="27" t="n">
+        <v>44563</v>
+      </c>
+      <c r="AL1" s="27" t="n">
+        <v>44564</v>
+      </c>
+      <c r="AM1" s="27" t="n">
+        <v>44565</v>
+      </c>
+      <c r="AN1" s="27" t="n">
+        <v>44566</v>
+      </c>
+      <c r="AO1" s="28" t="n">
+        <v>44567</v>
+      </c>
+      <c r="AP1" s="27" t="n">
+        <v>44568</v>
+      </c>
+      <c r="AQ1" s="27" t="n">
+        <v>44569</v>
+      </c>
+      <c r="AR1" s="27" t="n">
+        <v>44570</v>
+      </c>
+      <c r="AS1" s="27" t="n">
+        <v>44571</v>
+      </c>
+      <c r="AT1" s="27" t="n">
+        <v>44572</v>
+      </c>
+      <c r="AU1" s="27" t="n">
+        <v>44573</v>
+      </c>
+      <c r="AV1" s="27" t="n">
+        <v>44574</v>
+      </c>
+      <c r="AW1" s="27" t="n">
+        <v>44575</v>
+      </c>
+      <c r="AX1" s="27" t="n">
+        <v>44576</v>
+      </c>
+      <c r="AY1" s="27" t="n">
+        <v>44577</v>
+      </c>
+      <c r="AZ1" s="27" t="n">
+        <v>44578</v>
+      </c>
+      <c r="BA1" s="27" t="n">
+        <v>44579</v>
+      </c>
+      <c r="BB1" s="27" t="n">
+        <v>44580</v>
+      </c>
+      <c r="BC1" s="27" t="n">
+        <v>44581</v>
+      </c>
+      <c r="BD1" s="27" t="n">
+        <v>44582</v>
+      </c>
+      <c r="BE1" s="27" t="n">
+        <v>44583</v>
+      </c>
+      <c r="BF1" s="27" t="n">
+        <v>44584</v>
+      </c>
+      <c r="BG1" s="27" t="n">
+        <v>44585</v>
+      </c>
+      <c r="BH1" s="27" t="n">
+        <v>44586</v>
+      </c>
+      <c r="BI1" s="27" t="n">
+        <v>44587</v>
+      </c>
+      <c r="BJ1" s="27" t="n">
+        <v>44588</v>
+      </c>
+      <c r="BK1" s="27" t="n">
+        <v>44589</v>
+      </c>
+      <c r="BL1" s="27" t="n">
+        <v>44590</v>
+      </c>
+      <c r="BM1" s="27" t="n">
+        <v>44591</v>
+      </c>
+      <c r="BN1" s="27" t="n">
+        <v>44592</v>
+      </c>
+      <c r="BO1" s="27" t="n">
+        <v>44593</v>
+      </c>
+      <c r="BP1" s="27" t="n">
+        <v>44594</v>
+      </c>
+      <c r="BQ1" s="27" t="n">
+        <v>44595</v>
+      </c>
+      <c r="BR1" s="27" t="n">
+        <v>44596</v>
+      </c>
+      <c r="BS1" s="27" t="n">
+        <v>44597</v>
+      </c>
+      <c r="BT1" s="27" t="n">
+        <v>44598</v>
+      </c>
+      <c r="BU1" s="27" t="n">
+        <v>44599</v>
+      </c>
+      <c r="BV1" s="27" t="n">
+        <v>44600</v>
+      </c>
+      <c r="BW1" s="27" t="n">
+        <v>44601</v>
+      </c>
+      <c r="BX1" s="27" t="n">
+        <v>44602</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2922,6 +3177,13 @@
       <c r="H2" s="2" t="n">
         <v>6</v>
       </c>
+      <c r="I2" s="29" t="n">
+        <f aca="false">SUM(J2:FF2)</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AO2" s="30"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -2940,6 +3202,10 @@
       <c r="H3" s="2" t="n">
         <v>7</v>
       </c>
+      <c r="I3" s="29"/>
+      <c r="AB3" s="30"/>
+      <c r="AI3" s="30"/>
+      <c r="AO3" s="30"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -2960,6 +3226,10 @@
       <c r="H4" s="2" t="n">
         <v>7</v>
       </c>
+      <c r="I4" s="29"/>
+      <c r="AB4" s="30"/>
+      <c r="AI4" s="30"/>
+      <c r="AO4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -2978,6 +3248,10 @@
       <c r="H5" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="I5" s="29"/>
+      <c r="AB5" s="30"/>
+      <c r="AI5" s="30"/>
+      <c r="AO5" s="30"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -2996,6 +3270,10 @@
       <c r="H6" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="I6" s="29"/>
+      <c r="AB6" s="30"/>
+      <c r="AI6" s="30"/>
+      <c r="AO6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -3014,6 +3292,10 @@
       <c r="H7" s="2" t="n">
         <v>5</v>
       </c>
+      <c r="I7" s="29"/>
+      <c r="AB7" s="30"/>
+      <c r="AI7" s="30"/>
+      <c r="AO7" s="30"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -3036,6 +3318,10 @@
       <c r="H8" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="I8" s="29"/>
+      <c r="AB8" s="30"/>
+      <c r="AI8" s="30"/>
+      <c r="AO8" s="30"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -3060,6 +3346,10 @@
       <c r="H9" s="2" t="n">
         <v>6</v>
       </c>
+      <c r="I9" s="29"/>
+      <c r="AB9" s="30"/>
+      <c r="AI9" s="30"/>
+      <c r="AO9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
@@ -3078,6 +3368,10 @@
       <c r="H10" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="I10" s="29"/>
+      <c r="AB10" s="30"/>
+      <c r="AI10" s="30"/>
+      <c r="AO10" s="30"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
@@ -3098,6 +3392,10 @@
       <c r="H11" s="2" t="n">
         <v>8</v>
       </c>
+      <c r="I11" s="29"/>
+      <c r="AB11" s="30"/>
+      <c r="AI11" s="30"/>
+      <c r="AO11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
@@ -3116,6 +3414,10 @@
       <c r="H12" s="2" t="n">
         <v>9</v>
       </c>
+      <c r="I12" s="29"/>
+      <c r="AB12" s="30"/>
+      <c r="AI12" s="30"/>
+      <c r="AO12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
@@ -3136,28 +3438,65 @@
       <c r="H13" s="2" t="n">
         <v>8</v>
       </c>
+      <c r="I13" s="29"/>
+      <c r="AB13" s="30"/>
+      <c r="AI13" s="30"/>
+      <c r="AO13" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <v>0</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="F15" s="6"/>
+      <c r="C15" s="8" t="n">
+        <f aca="false">A15+A17</f>
+        <v>6</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <f aca="false">C15</f>
+        <v>6</v>
+      </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="8"/>
-      <c r="K15" s="6"/>
+      <c r="H15" s="8" t="n">
+        <f aca="false">F15+F17</f>
+        <v>13</v>
+      </c>
+      <c r="K15" s="6" t="n">
+        <f aca="false">H15</f>
+        <v>13</v>
+      </c>
       <c r="L15" s="7"/>
-      <c r="M15" s="8"/>
-      <c r="P15" s="6"/>
+      <c r="M15" s="8" t="n">
+        <f aca="false">K15+K17</f>
+        <v>17</v>
+      </c>
+      <c r="P15" s="6" t="n">
+        <f aca="false">M15</f>
+        <v>17</v>
+      </c>
       <c r="Q15" s="7"/>
-      <c r="R15" s="8"/>
-      <c r="U15" s="6"/>
+      <c r="R15" s="8" t="n">
+        <f aca="false">P15+P17</f>
+        <v>20</v>
+      </c>
+      <c r="U15" s="6" t="n">
+        <f aca="false">R15</f>
+        <v>20</v>
+      </c>
       <c r="V15" s="7"/>
-      <c r="W15" s="8"/>
-      <c r="Z15" s="6"/>
+      <c r="W15" s="8" t="n">
+        <f aca="false">U15+U17</f>
+        <v>28</v>
+      </c>
+      <c r="Z15" s="6" t="n">
+        <f aca="false">MAX(W15,W20,W25)</f>
+        <v>33</v>
+      </c>
       <c r="AA15" s="7"/>
-      <c r="AB15" s="8"/>
+      <c r="AB15" s="8" t="n">
+        <f aca="false">Z15+Z17</f>
+        <v>41</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
@@ -3191,73 +3530,166 @@
       <c r="AA16" s="9"/>
       <c r="AB16" s="9"/>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="n">
         <f aca="false">H2</f>
         <v>6</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="11"/>
+      <c r="B17" s="31" t="n">
+        <f aca="false">C18-C15</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="11" t="n">
+        <f aca="false">MIN(F15,F20)-C15</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="10" t="n">
         <f aca="false">H3</f>
         <v>7</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="G17" s="31" t="n">
+        <f aca="false">H18-H15</f>
+        <v>5</v>
+      </c>
+      <c r="H17" s="11" t="n">
+        <f aca="false">K15-H15</f>
+        <v>0</v>
+      </c>
       <c r="K17" s="10" t="n">
         <f aca="false">H5</f>
         <v>4</v>
       </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
+      <c r="L17" s="31" t="n">
+        <f aca="false">M18-M15</f>
+        <v>5</v>
+      </c>
+      <c r="M17" s="11" t="n">
+        <f aca="false">P15-M15</f>
+        <v>0</v>
+      </c>
       <c r="P17" s="10" t="n">
         <f aca="false">H8</f>
         <v>3</v>
       </c>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
+      <c r="Q17" s="31" t="n">
+        <f aca="false">R18-R15</f>
+        <v>5</v>
+      </c>
+      <c r="R17" s="11" t="n">
+        <f aca="false">U15-R15</f>
+        <v>0</v>
+      </c>
       <c r="U17" s="10" t="n">
         <f aca="false">H11</f>
         <v>8</v>
       </c>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
+      <c r="V17" s="31" t="n">
+        <f aca="false">W18-W15</f>
+        <v>5</v>
+      </c>
+      <c r="W17" s="11" t="n">
+        <f aca="false">Z15-W15</f>
+        <v>5</v>
+      </c>
       <c r="Z17" s="10" t="n">
         <f aca="false">H13</f>
         <v>8</v>
       </c>
-      <c r="AA17" s="11"/>
+      <c r="AA17" s="31" t="n">
+        <f aca="false">AB18-AB15</f>
+        <v>0</v>
+      </c>
       <c r="AB17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
+      <c r="A18" s="12" t="n">
+        <f aca="false">C18-A17</f>
+        <v>0</v>
+      </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="F18" s="12"/>
+      <c r="C18" s="14" t="n">
+        <f aca="false">MIN(F18,F23)</f>
+        <v>6</v>
+      </c>
+      <c r="F18" s="12" t="n">
+        <f aca="false">H18-F17</f>
+        <v>11</v>
+      </c>
       <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="K18" s="12"/>
+      <c r="H18" s="14" t="n">
+        <f aca="false">K18</f>
+        <v>18</v>
+      </c>
+      <c r="K18" s="12" t="n">
+        <f aca="false">M18-K17</f>
+        <v>18</v>
+      </c>
       <c r="L18" s="13"/>
-      <c r="M18" s="14"/>
-      <c r="P18" s="12"/>
+      <c r="M18" s="14" t="n">
+        <f aca="false">P18</f>
+        <v>22</v>
+      </c>
+      <c r="P18" s="12" t="n">
+        <f aca="false">R18-P17</f>
+        <v>22</v>
+      </c>
       <c r="Q18" s="13"/>
-      <c r="R18" s="14"/>
-      <c r="U18" s="12"/>
+      <c r="R18" s="14" t="n">
+        <f aca="false">U18</f>
+        <v>25</v>
+      </c>
+      <c r="U18" s="12" t="n">
+        <f aca="false">W18-U17</f>
+        <v>25</v>
+      </c>
       <c r="V18" s="13"/>
-      <c r="W18" s="14"/>
-      <c r="Z18" s="12"/>
+      <c r="W18" s="14" t="n">
+        <f aca="false">Z18</f>
+        <v>33</v>
+      </c>
+      <c r="Z18" s="12" t="n">
+        <f aca="false">AB18-Z17</f>
+        <v>33</v>
+      </c>
       <c r="AA18" s="13"/>
-      <c r="AB18" s="14"/>
+      <c r="AB18" s="14" t="n">
+        <f aca="false">AB15</f>
+        <v>41</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="6"/>
-      <c r="H20" s="8"/>
-      <c r="K20" s="6"/>
-      <c r="M20" s="8"/>
-      <c r="P20" s="6"/>
-      <c r="R20" s="8"/>
-      <c r="U20" s="6"/>
-      <c r="W20" s="8"/>
+      <c r="F20" s="6" t="n">
+        <f aca="false">C15</f>
+        <v>6</v>
+      </c>
+      <c r="H20" s="8" t="n">
+        <f aca="false">F20+F22</f>
+        <v>13</v>
+      </c>
+      <c r="K20" s="6" t="n">
+        <f aca="false">H20</f>
+        <v>13</v>
+      </c>
+      <c r="M20" s="8" t="n">
+        <f aca="false">K20+K22</f>
+        <v>17</v>
+      </c>
+      <c r="P20" s="6" t="n">
+        <f aca="false">MAX(M20,M25)</f>
+        <v>18</v>
+      </c>
+      <c r="R20" s="8" t="n">
+        <f aca="false">P20+P22</f>
+        <v>24</v>
+      </c>
+      <c r="U20" s="6" t="n">
+        <f aca="false">R20</f>
+        <v>24</v>
+      </c>
+      <c r="W20" s="8" t="n">
+        <f aca="false">U20+U22</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="9" t="s">
@@ -3281,51 +3713,111 @@
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F22" s="10" t="n">
         <f aca="false">H4</f>
         <v>7</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="G22" s="31" t="n">
+        <f aca="false">H23-H20</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="11" t="n">
+        <f aca="false">MIN(K20,K25)-H20</f>
+        <v>0</v>
+      </c>
       <c r="K22" s="10" t="n">
         <f aca="false">H6</f>
         <v>4</v>
       </c>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
+      <c r="L22" s="31" t="n">
+        <f aca="false">M23-M20</f>
+        <v>1</v>
+      </c>
+      <c r="M22" s="11" t="n">
+        <f aca="false">P20-M20</f>
+        <v>1</v>
+      </c>
       <c r="P22" s="10" t="n">
         <f aca="false">H9</f>
         <v>6</v>
       </c>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
+      <c r="Q22" s="31" t="n">
+        <f aca="false">R23-R20</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="11" t="n">
+        <f aca="false">MIN(U20,U25)-R20</f>
+        <v>0</v>
+      </c>
       <c r="U22" s="10" t="n">
         <f aca="false">H10</f>
         <v>2</v>
       </c>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
+      <c r="V22" s="31" t="n">
+        <f aca="false">W23-W20</f>
+        <v>7</v>
+      </c>
+      <c r="W22" s="11" t="n">
+        <f aca="false">Z15-W20</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="12"/>
+      <c r="F23" s="12" t="n">
+        <f aca="false">H23-F22</f>
+        <v>6</v>
+      </c>
       <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="K23" s="12"/>
+      <c r="H23" s="14" t="n">
+        <f aca="false">MIN(K23,K28)</f>
+        <v>13</v>
+      </c>
+      <c r="K23" s="12" t="n">
+        <f aca="false">M23-K22</f>
+        <v>14</v>
+      </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="14"/>
-      <c r="P23" s="12"/>
+      <c r="M23" s="14" t="n">
+        <f aca="false">P23</f>
+        <v>18</v>
+      </c>
+      <c r="P23" s="12" t="n">
+        <f aca="false">R23-P22</f>
+        <v>18</v>
+      </c>
       <c r="Q23" s="13"/>
-      <c r="R23" s="14"/>
-      <c r="U23" s="12"/>
+      <c r="R23" s="14" t="n">
+        <f aca="false">MIN(U23,U28)</f>
+        <v>24</v>
+      </c>
+      <c r="U23" s="12" t="n">
+        <f aca="false">W23-U22</f>
+        <v>31</v>
+      </c>
       <c r="V23" s="13"/>
-      <c r="W23" s="14"/>
+      <c r="W23" s="14" t="n">
+        <f aca="false">Z18</f>
+        <v>33</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K25" s="6"/>
-      <c r="M25" s="8"/>
-      <c r="U25" s="6"/>
-      <c r="W25" s="8"/>
+      <c r="K25" s="6" t="n">
+        <f aca="false">H20</f>
+        <v>13</v>
+      </c>
+      <c r="M25" s="8" t="n">
+        <f aca="false">K25+K27</f>
+        <v>18</v>
+      </c>
+      <c r="U25" s="6" t="n">
+        <f aca="false">R20</f>
+        <v>24</v>
+      </c>
+      <c r="W25" s="8" t="n">
+        <f aca="false">U25+U27</f>
+        <v>33</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K26" s="9" t="s">
@@ -3344,22 +3836,46 @@
         <f aca="false">H7</f>
         <v>5</v>
       </c>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
+      <c r="L27" s="31" t="n">
+        <f aca="false">M28-M25</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="11" t="n">
+        <f aca="false">P20-M25</f>
+        <v>0</v>
+      </c>
       <c r="U27" s="10" t="n">
         <f aca="false">H12</f>
         <v>9</v>
       </c>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
+      <c r="V27" s="31" t="n">
+        <f aca="false">W28-W25</f>
+        <v>0</v>
+      </c>
+      <c r="W27" s="11" t="n">
+        <f aca="false">Z15-W25</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K28" s="12"/>
+      <c r="K28" s="12" t="n">
+        <f aca="false">M28-K27</f>
+        <v>13</v>
+      </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="14"/>
-      <c r="U28" s="12"/>
+      <c r="M28" s="14" t="n">
+        <f aca="false">P23</f>
+        <v>18</v>
+      </c>
+      <c r="U28" s="12" t="n">
+        <f aca="false">W28-U27</f>
+        <v>24</v>
+      </c>
       <c r="V28" s="13"/>
-      <c r="W28" s="14"/>
+      <c r="W28" s="14" t="n">
+        <f aca="false">Z18</f>
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3393,9 +3909,14 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17 G17 G22 L17 L22 L27 Q17 Q22 V17 V22 V27 AA17">
+  <conditionalFormatting sqref="AA17 V17 V22 V27 Q22 Q17 L17 L22 L27 G22 G17 B17">
     <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:BX13">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>IF(OR(WEEKDAY(J$1)=7,WEEKDAY(J$1)=1),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>